<commit_message>
Various changes in Eurofer file
</commit_message>
<xml_diff>
--- a/Jupyter/Eurofer/Eurofer_data_1_1.xlsx
+++ b/Jupyter/Eurofer/Eurofer_data_1_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Research\Repos\DatabaseCodes\Jupyter\Eurofer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghoni/My Drive/Research/Repos/DatabaseCodes/Jupyter/Eurofer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2364363-68E0-4A55-BA52-0A4CAF7AA150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5E5DEC-AC36-524D-89B7-98DB46691229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="852" activeTab="12" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
+    <workbookView xWindow="4440" yWindow="760" windowWidth="24960" windowHeight="16900" tabRatio="852" firstSheet="3" activeTab="8" xr2:uid="{D289EE42-B074-4616-9B9B-4CE9F1662138}"/>
   </bookViews>
   <sheets>
     <sheet name="Density" sheetId="15" r:id="rId1"/>
@@ -830,6 +830,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -844,12 +850,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2187,13 +2187,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>34463</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2702,18 +2702,18 @@
       <selection activeCell="A45" sqref="A45:C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
-    </row>
-    <row r="3" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B1" s="19"/>
+    </row>
+    <row r="3" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>293</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>7750</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>373</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>7728</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>473</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>7699</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>573</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>7666</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>673</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>7633</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>773</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>7596</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>873</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>7558</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" ht="224" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
         <v>78</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="16"/>
       <c r="B46" s="16"/>
       <c r="C46" s="16"/>
@@ -2809,95 +2809,95 @@
       <selection activeCell="G25" sqref="G25:J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="32" width="12.6328125" style="2" customWidth="1"/>
-    <col min="33" max="33" width="3.26953125" style="2" customWidth="1"/>
-    <col min="34" max="34" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="3.54296875" style="2" customWidth="1"/>
-    <col min="37" max="37" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="2.1796875" style="2" customWidth="1"/>
-    <col min="40" max="40" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="3.54296875" style="2" customWidth="1"/>
-    <col min="43" max="43" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="32" width="12.6640625" style="2" customWidth="1"/>
+    <col min="33" max="33" width="3.33203125" style="2" customWidth="1"/>
+    <col min="34" max="34" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="3.5" style="2" customWidth="1"/>
+    <col min="37" max="37" width="5.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="2.1640625" style="2" customWidth="1"/>
+    <col min="40" max="40" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="3.5" style="2" customWidth="1"/>
+    <col min="43" max="43" width="5.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="5" style="2" customWidth="1"/>
-    <col min="46" max="46" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="3.54296875" style="2" customWidth="1"/>
-    <col min="49" max="49" width="5.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="3.1796875" style="2" customWidth="1"/>
-    <col min="52" max="52" width="5.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="12.54296875" style="2"/>
+    <col min="46" max="46" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="3.5" style="2" customWidth="1"/>
+    <col min="49" max="49" width="5.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="3.1640625" style="2" customWidth="1"/>
+    <col min="52" max="52" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="8.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="12.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:53" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17" t="s">
+      <c r="L1" s="19"/>
+      <c r="M1" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17" t="s">
+      <c r="N1" s="19"/>
+      <c r="O1" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17" t="s">
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17" t="s">
+      <c r="R1" s="19"/>
+      <c r="S1" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="T1" s="17"/>
+      <c r="T1" s="19"/>
       <c r="U1" s="11"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
       <c r="AA1" s="11"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
+      <c r="AB1" s="19"/>
+      <c r="AC1" s="19"/>
       <c r="AG1" s="11"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="17"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
       <c r="AM1" s="11"/>
-      <c r="AN1" s="17"/>
-      <c r="AO1" s="17"/>
+      <c r="AN1" s="19"/>
+      <c r="AO1" s="19"/>
       <c r="AS1" s="11"/>
-      <c r="AT1" s="17"/>
-      <c r="AU1" s="17"/>
+      <c r="AT1" s="19"/>
+      <c r="AU1" s="19"/>
       <c r="AY1" s="11"/>
-      <c r="AZ1" s="17"/>
-      <c r="BA1" s="17"/>
-    </row>
-    <row r="2" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:53" ht="29" x14ac:dyDescent="0.35">
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="19"/>
+    </row>
+    <row r="2" spans="1:53" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:53" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>20</v>
       </c>
@@ -3044,7 +3044,7 @@
       <c r="AZ4" s="14"/>
       <c r="BA4" s="14"/>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>50</v>
       </c>
@@ -3129,7 +3129,7 @@
       <c r="AZ5" s="14"/>
       <c r="BA5" s="14"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>100</v>
       </c>
@@ -3214,7 +3214,7 @@
       <c r="AZ6" s="14"/>
       <c r="BA6" s="14"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>150</v>
       </c>
@@ -3297,7 +3297,7 @@
       <c r="AZ7" s="14"/>
       <c r="BA7" s="14"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>200</v>
       </c>
@@ -3380,7 +3380,7 @@
       <c r="AZ8" s="14"/>
       <c r="BA8" s="14"/>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>250</v>
       </c>
@@ -3439,7 +3439,7 @@
       <c r="AZ9" s="15"/>
       <c r="BA9" s="15"/>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>300</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>427.45071999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>350</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>410.36381999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>400</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>388.04959000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>450</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>353.96629000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>500</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>310.73838999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>550</v>
       </c>
@@ -3523,7 +3523,7 @@
         <v>253.12702999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>600</v>
       </c>
@@ -3537,7 +3537,7 @@
         <v>178.52502999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>650</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>81.697839999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>700</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>137.14859437750999</v>
       </c>
     </row>
-    <row r="23" spans="1:53" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:53" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>85</v>
       </c>
@@ -3570,72 +3570,78 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:53" ht="152.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:53" ht="152.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="17"/>
+      <c r="B25" s="19"/>
       <c r="C25" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="17"/>
-      <c r="V25" s="17"/>
-      <c r="W25" s="17"/>
-      <c r="X25" s="17"/>
-      <c r="Y25" s="17"/>
-      <c r="Z25" s="17"/>
-      <c r="AA25" s="17"/>
-      <c r="AB25" s="17"/>
-      <c r="AC25" s="17"/>
-      <c r="AD25" s="17"/>
-      <c r="AE25" s="17"/>
-      <c r="AF25" s="17"/>
-      <c r="AG25" s="17"/>
-      <c r="AH25" s="17"/>
-      <c r="AI25" s="17"/>
-      <c r="AJ25" s="17"/>
-      <c r="AK25" s="17"/>
-      <c r="AL25" s="17"/>
-      <c r="AM25" s="17"/>
-      <c r="AN25" s="17"/>
-      <c r="AO25" s="17"/>
-      <c r="AP25" s="17"/>
-      <c r="AQ25" s="17"/>
-      <c r="AR25" s="17"/>
-      <c r="AS25" s="17"/>
-      <c r="AT25" s="17"/>
-      <c r="AU25" s="17"/>
-      <c r="AV25" s="17"/>
-      <c r="AW25" s="17"/>
-      <c r="AX25" s="17"/>
-      <c r="AY25" s="17"/>
-      <c r="AZ25" s="17"/>
-      <c r="BA25" s="17"/>
-    </row>
-    <row r="26" spans="1:53" ht="29" x14ac:dyDescent="0.35">
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+      <c r="W25" s="19"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="19"/>
+      <c r="Z25" s="19"/>
+      <c r="AA25" s="19"/>
+      <c r="AB25" s="19"/>
+      <c r="AC25" s="19"/>
+      <c r="AD25" s="19"/>
+      <c r="AE25" s="19"/>
+      <c r="AF25" s="19"/>
+      <c r="AG25" s="19"/>
+      <c r="AH25" s="19"/>
+      <c r="AI25" s="19"/>
+      <c r="AJ25" s="19"/>
+      <c r="AK25" s="19"/>
+      <c r="AL25" s="19"/>
+      <c r="AM25" s="19"/>
+      <c r="AN25" s="19"/>
+      <c r="AO25" s="19"/>
+      <c r="AP25" s="19"/>
+      <c r="AQ25" s="19"/>
+      <c r="AR25" s="19"/>
+      <c r="AS25" s="19"/>
+      <c r="AT25" s="19"/>
+      <c r="AU25" s="19"/>
+      <c r="AV25" s="19"/>
+      <c r="AW25" s="19"/>
+      <c r="AX25" s="19"/>
+      <c r="AY25" s="19"/>
+      <c r="AZ25" s="19"/>
+      <c r="BA25" s="19"/>
+    </row>
+    <row r="26" spans="1:53" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="K25:BA25"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
@@ -3644,12 +3650,6 @@
     <mergeCell ref="AT1:AU1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="AB1:AC1"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="AH1:AI1"/>
@@ -3675,52 +3675,52 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="12.6328125" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="12.54296875" style="2"/>
+    <col min="1" max="26" width="12.6640625" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="12.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:18" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="F1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17" t="s">
+      <c r="H1" s="19"/>
+      <c r="I1" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17" t="s">
+      <c r="L1" s="19"/>
+      <c r="M1" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17" t="s">
+      <c r="N1" s="19"/>
+      <c r="O1" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17" t="s">
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="R1" s="17"/>
-    </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+      <c r="R1" s="19"/>
+    </row>
+    <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:18" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -3776,7 +3776,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>20</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>621.67832167832103</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>100</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>505.233380480905</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>150</v>
       </c>
@@ -3944,7 +3944,7 @@
         <v>475.53041018387501</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>200</v>
       </c>
@@ -3996,7 +3996,7 @@
         <v>399.15134370579898</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>250</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>282.46110325318199</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>300</v>
       </c>
@@ -4076,7 +4076,7 @@
       <c r="Q9" s="15"/>
       <c r="R9" s="15"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>350</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>495.42626000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>400</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>466.57317999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>450</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>432.49275</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>500</v>
       </c>
@@ -4108,7 +4108,7 @@
         <v>389.26197000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>550</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>339.49808999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>600</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>276.65652999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>650</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>199.44013000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>700</v>
       </c>
@@ -4140,21 +4140,23 @@
         <v>105.22734</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="G21" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
@@ -4162,8 +4164,6 @@
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="O1:P1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B22" r:id="rId1" xr:uid="{49CE8F48-BC1C-42DF-8D69-1569F2C329D5}"/>
@@ -4182,32 +4182,32 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="12.54296875" style="1"/>
+    <col min="1" max="16384" width="12.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="20"/>
+      <c r="D1" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="J1" s="18" t="s">
+      <c r="H1" s="19"/>
+      <c r="J1" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="18"/>
+      <c r="K1" s="20"/>
       <c r="L1" s="10"/>
     </row>
-    <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4236,7 +4236,7 @@
       </c>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -4265,7 +4265,7 @@
       </c>
       <c r="L4"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>50</v>
       </c>
@@ -4294,7 +4294,7 @@
       </c>
       <c r="L5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>100</v>
       </c>
@@ -4324,7 +4324,7 @@
       <c r="L6"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>150</v>
       </c>
@@ -4354,7 +4354,7 @@
       <c r="L7"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>200</v>
       </c>
@@ -4384,7 +4384,7 @@
       <c r="L8"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>250</v>
       </c>
@@ -4414,7 +4414,7 @@
       <c r="L9"/>
       <c r="M9" s="10"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>300</v>
       </c>
@@ -4437,7 +4437,7 @@
       <c r="L10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>350</v>
       </c>
@@ -4450,7 +4450,7 @@
       <c r="L11"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>400</v>
       </c>
@@ -4463,7 +4463,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>450</v>
       </c>
@@ -4476,7 +4476,7 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>500</v>
       </c>
@@ -4489,7 +4489,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>550</v>
       </c>
@@ -4502,7 +4502,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>600</v>
       </c>
@@ -4511,7 +4511,7 @@
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>650</v>
       </c>
@@ -4520,7 +4520,7 @@
       </c>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>700</v>
       </c>
@@ -4529,32 +4529,32 @@
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="41" spans="1:13" ht="84.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="17" t="s">
+    <row r="41" spans="1:13" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="17"/>
+      <c r="B41" s="19"/>
       <c r="C41" s="11"/>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
-      <c r="G41" s="18"/>
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18"/>
-      <c r="M41" s="18"/>
-    </row>
-    <row r="42" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="21" t="s">
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="20"/>
+    </row>
+    <row r="42" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="23"/>
       <c r="C42" s="7"/>
-      <c r="G42" s="23" t="s">
+      <c r="G42" s="18" t="s">
         <v>109</v>
       </c>
     </row>
@@ -4582,36 +4582,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05EE98D8-EC6F-4F75-B479-0C3190D73C5A}">
   <dimension ref="A1:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="44" width="12.6328125" customWidth="1"/>
+    <col min="4" max="44" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:11" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="19"/>
       <c r="F1" s="10"/>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="19"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="K1" s="18"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K1" s="20"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="D2" s="1"/>
@@ -4623,7 +4623,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20.392552617942201</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>7.4201574324111004</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>98.942940742330407</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>9.0969876631072601</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>199.54662465257201</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>3.4768285088688402</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>302.77768297853402</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>2.9100603500474902</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>400.23541850958202</v>
       </c>
@@ -4774,7 +4774,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>501.76235167262502</v>
       </c>
@@ -4793,7 +4793,7 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>600.21737059467102</v>
       </c>
@@ -4812,7 +4812,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -4822,7 +4822,7 @@
       <c r="J11" s="10"/>
       <c r="K11" s="10"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -4832,7 +4832,7 @@
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -4842,7 +4842,7 @@
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -4852,7 +4852,7 @@
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -4862,35 +4862,35 @@
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B43" s="17" t="s">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B43" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="17"/>
+      <c r="C43" s="19"/>
       <c r="F43" s="11"/>
-      <c r="G43" s="18" t="s">
+      <c r="G43" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="H43" s="18"/>
-      <c r="I43" s="18"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18"/>
-      <c r="M43" s="18"/>
-      <c r="N43" s="18"/>
-      <c r="O43" s="18"/>
-      <c r="P43" s="18"/>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B44" s="21" t="s">
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="20"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B44" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="21"/>
+      <c r="C44" s="23"/>
       <c r="F44" s="7"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="23" t="s">
+      <c r="J44" s="18" t="s">
         <v>109</v>
       </c>
       <c r="K44" s="1"/>
@@ -4928,43 +4928,43 @@
       <selection activeCell="T35" sqref="T35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="18" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="9.1640625" style="2"/>
     <col min="4" max="5" width="18" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="2"/>
+    <col min="6" max="6" width="9.1640625" style="2"/>
     <col min="7" max="8" width="18" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="2"/>
+    <col min="9" max="9" width="9.1640625" style="2"/>
     <col min="10" max="11" width="18" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11.26953125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="2" customWidth="1"/>
     <col min="13" max="14" width="18" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="2"/>
+    <col min="15" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="J1" s="17" t="s">
+      <c r="H1" s="19"/>
+      <c r="J1" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="M1" s="17" t="s">
+      <c r="K1" s="19"/>
+      <c r="M1" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="N1" s="17"/>
-    </row>
-    <row r="3" spans="1:14" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="N1" s="19"/>
+    </row>
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>-195.475113122171</v>
       </c>
@@ -5028,7 +5028,7 @@
         <v>13.2227855651655</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>-52.4886877828054</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>155.23173277661701</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>-22.624434389140202</v>
       </c>
@@ -5092,7 +5092,7 @@
         <v>164.140769460184</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>-3.6199095022624301</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>170.56606024455701</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>20.814479638009001</v>
       </c>
@@ -5156,7 +5156,7 @@
         <v>195.45600954369201</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>200.90497737556501</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>180.121682075753</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>400</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>196.49865791828199</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G11" s="1">
         <v>22.743215031315199</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>267.01938562481303</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G12" s="1">
         <v>39.774530271398703</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>267.12078735460699</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G13" s="1">
         <v>59.986877423203097</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>269.22039964211098</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G14" s="1">
         <v>70.293468535639704</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>276.25171488219502</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M15" s="1">
         <v>60.0960334029227</v>
       </c>
@@ -5302,7 +5302,7 @@
         <v>300.66925141664098</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="M16" s="1">
         <v>59.741723829406503</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>248.06203399940301</v>
       </c>
     </row>
-    <row r="17" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M17" s="1">
         <v>-80.320906650760506</v>
       </c>
@@ -5318,7 +5318,7 @@
         <v>14.116313748881501</v>
       </c>
     </row>
-    <row r="18" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M18" s="1">
         <v>-70.226066209364703</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>14.662690128243399</v>
       </c>
     </row>
-    <row r="19" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M19" s="1">
         <v>-60.384730092454497</v>
       </c>
@@ -5334,7 +5334,7 @@
         <v>20.6668654935878</v>
       </c>
     </row>
-    <row r="20" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M20" s="1">
         <v>-50.168207575305701</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>170.593498359677</v>
       </c>
     </row>
-    <row r="21" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M21" s="1">
         <v>-40.341186996719301</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>182.55293766776001</v>
       </c>
     </row>
-    <row r="22" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M22" s="1">
         <v>-19.960035788845801</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>203.994035192365</v>
       </c>
     </row>
-    <row r="23" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M23" s="1">
         <v>-7.8735460781359706E-2</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>233.37309871756599</v>
       </c>
     </row>
-    <row r="24" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M24" s="1">
         <v>23.428571428571399</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>254.33343274679299</v>
       </c>
     </row>
-    <row r="25" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M25" s="1">
         <v>39.994631673128502</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>262.85237101103399</v>
       </c>
     </row>
-    <row r="26" spans="13:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="13:14" x14ac:dyDescent="0.2">
       <c r="M26" s="1">
         <v>60.162839248434203</v>
       </c>
@@ -5390,24 +5390,24 @@
         <v>272.87801968386498</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="17" t="s">
+    <row r="36" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="17"/>
-      <c r="C36" s="17"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="17"/>
-      <c r="G36" s="17" t="s">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="G36" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -5432,48 +5432,48 @@
       <selection activeCell="M34" sqref="M34:N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="2"/>
-    <col min="4" max="4" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="2"/>
+    <col min="4" max="4" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="2"/>
-    <col min="7" max="7" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="2"/>
-    <col min="10" max="10" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="2"/>
+    <col min="7" max="7" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="2"/>
+    <col min="10" max="10" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="2"/>
+    <col min="15" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="J1" s="17" t="s">
+      <c r="H1" s="19"/>
+      <c r="J1" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="M1" s="17" t="s">
+      <c r="K1" s="19"/>
+      <c r="M1" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="17"/>
-    </row>
-    <row r="3" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="N1" s="19"/>
+    </row>
+    <row r="3" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -5505,7 +5505,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>10</v>
       </c>
@@ -5537,7 +5537,7 @@
         <v>95.557891687808393</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>30</v>
       </c>
@@ -5569,7 +5569,7 @@
         <v>88.682804290936701</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>100</v>
       </c>
@@ -5601,7 +5601,7 @@
         <v>81.200483429553103</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>300</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>74.529005773187606</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>1000</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>66.640813839669093</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>3000</v>
       </c>
@@ -5697,7 +5697,7 @@
         <v>60.172496454184</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>10000</v>
       </c>
@@ -5729,7 +5729,7 @@
         <v>52.487914261171703</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>30000</v>
       </c>
@@ -5761,7 +5761,7 @@
         <v>45.612377394674198</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>100000</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>37.927795201662001</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>300000</v>
       </c>
@@ -5825,37 +5825,37 @@
         <v>30.849547533909899</v>
       </c>
     </row>
-    <row r="32" spans="13:23" x14ac:dyDescent="0.35">
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="17"/>
-      <c r="V32" s="17"/>
-      <c r="W32" s="17"/>
-    </row>
-    <row r="34" spans="1:23" ht="147" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="17" t="s">
+    <row r="32" spans="13:23" x14ac:dyDescent="0.2">
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+    </row>
+    <row r="34" spans="1:23" ht="147" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="M34" s="17" t="s">
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="M34" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="N34" s="17"/>
+      <c r="N34" s="19"/>
       <c r="O34" s="11"/>
       <c r="P34" s="11"/>
       <c r="Q34" s="11"/>
@@ -5891,55 +5891,55 @@
       <selection activeCell="P52" sqref="P52:T52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="13.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="2" customWidth="1"/>
-    <col min="4" max="5" width="13.453125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.1796875" style="2"/>
-    <col min="7" max="8" width="13.81640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="2"/>
-    <col min="10" max="11" width="14.453125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="9.1796875" style="2"/>
-    <col min="13" max="14" width="14.7265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="9.1796875" style="2"/>
-    <col min="16" max="17" width="15.26953125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="9.1796875" style="2"/>
-    <col min="19" max="20" width="15.26953125" style="2" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="2" width="13.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="2" customWidth="1"/>
+    <col min="4" max="5" width="13.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="2"/>
+    <col min="7" max="8" width="13.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="2"/>
+    <col min="10" max="11" width="14.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="2"/>
+    <col min="13" max="14" width="14.6640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.1640625" style="2"/>
+    <col min="16" max="17" width="15.33203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="9.1640625" style="2"/>
+    <col min="19" max="20" width="15.33203125" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="J1" s="17" t="s">
+      <c r="H1" s="19"/>
+      <c r="J1" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="17"/>
-      <c r="M1" s="17" t="s">
+      <c r="K1" s="19"/>
+      <c r="M1" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="17"/>
-      <c r="P1" s="17" t="s">
+      <c r="N1" s="19"/>
+      <c r="P1" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="17"/>
-      <c r="S1" s="17" t="s">
+      <c r="Q1" s="19"/>
+      <c r="S1" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="T1" s="17"/>
-    </row>
-    <row r="3" spans="1:20" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="T1" s="19"/>
+    </row>
+    <row r="3" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
@@ -5983,7 +5983,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>4.8638199999999996</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>1.81249999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>9.9451300000000007</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>1.61029411764705</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>24.994789999999998</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>48.371310000000001</v>
       </c>
@@ -6159,7 +6159,7 @@
         <v>1.4117647058823499</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>100.27548</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>1.41911764705882</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>252.01924</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>1.41911764705882</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>494.47662000000003</v>
       </c>
@@ -6291,7 +6291,7 @@
         <v>1.4117647058823499</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>50270.617209999997</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>1.40808823529411</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>98633.9179</v>
       </c>
@@ -6373,7 +6373,7 @@
         <v>1.2242647058823499</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>207303.64079999999</v>
       </c>
@@ -6411,7 +6411,7 @@
         <v>1.01838235294117</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>506872.17005999997</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>0.91911764705882304</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>1000000</v>
       </c>
@@ -6475,7 +6475,7 @@
         <v>0.91544117647058798</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="D16" s="2">
         <v>1008287.14299</v>
       </c>
@@ -6495,7 +6495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P17">
         <v>1608.5055696074701</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P18">
         <v>1254.92984463937</v>
       </c>
@@ -6523,7 +6523,7 @@
         <v>0.81617647058823495</v>
       </c>
     </row>
-    <row r="19" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P19">
         <v>1352.9212213830299</v>
       </c>
@@ -6537,7 +6537,7 @@
         <v>0.81617647058823495</v>
       </c>
     </row>
-    <row r="20" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P20">
         <v>1472.54042762412</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="21" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P21">
         <v>1528.95166956412</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>0.81985294117647001</v>
       </c>
     </row>
-    <row r="22" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P22">
         <v>1663.9047110839299</v>
       </c>
@@ -6579,7 +6579,7 @@
         <v>0.8125</v>
       </c>
     </row>
-    <row r="23" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P23">
         <v>1551.94508748353</v>
       </c>
@@ -6593,7 +6593,7 @@
         <v>0.66176470588235303</v>
       </c>
     </row>
-    <row r="24" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P24">
         <v>2156.4207065729001</v>
       </c>
@@ -6607,7 +6607,7 @@
         <v>0.60294117647058798</v>
       </c>
     </row>
-    <row r="25" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P25">
         <v>2273.3309522936602</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>0.39705882352941102</v>
       </c>
     </row>
-    <row r="26" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P26">
         <v>2450.8443254601498</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>0.51102941176470495</v>
       </c>
     </row>
-    <row r="27" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P27">
         <v>3099.5348132387398</v>
       </c>
@@ -6649,7 +6649,7 @@
         <v>0.51102941176470495</v>
       </c>
     </row>
-    <row r="28" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P28">
         <v>5296.0195526859297</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>0.51102941176470495</v>
       </c>
     </row>
-    <row r="29" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P29">
         <v>5090.0575080803101</v>
       </c>
@@ -6671,7 +6671,7 @@
         <v>0.54411764705882304</v>
       </c>
     </row>
-    <row r="30" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P30">
         <v>5324.6432593392001</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>0.49264705882352899</v>
       </c>
     </row>
-    <row r="31" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P31">
         <v>7126.5797989979101</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>0.496323529411764</v>
       </c>
     </row>
-    <row r="32" spans="16:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="16:20" x14ac:dyDescent="0.2">
       <c r="P32">
         <v>8205.51119349898</v>
       </c>
@@ -6695,7 +6695,7 @@
         <v>0.496323529411764</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P33">
         <v>12154.970287534299</v>
       </c>
@@ -6703,7 +6703,7 @@
         <v>0.44852941176470501</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="P34">
         <v>25018.3868587463</v>
       </c>
@@ -6711,33 +6711,33 @@
         <v>0.40073529411764702</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="88.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="17" t="s">
+    <row r="39" spans="1:17" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="G39" s="17" t="s">
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="G39" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-    </row>
-    <row r="52" spans="16:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="P52" s="17" t="s">
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+    </row>
+    <row r="52" spans="16:20" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P52" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="Q52" s="17"/>
-      <c r="R52" s="17"/>
-      <c r="S52" s="17"/>
-      <c r="T52" s="17"/>
+      <c r="Q52" s="19"/>
+      <c r="R52" s="19"/>
+      <c r="S52" s="19"/>
+      <c r="T52" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -6766,7 +6766,7 @@
       <selection activeCell="Q43" sqref="Q43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6780,27 +6780,27 @@
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="12.54296875" style="10" customWidth="1"/>
-    <col min="27" max="16384" width="8.81640625" style="10"/>
+    <col min="1" max="26" width="12.5" style="10" customWidth="1"/>
+    <col min="27" max="16384" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="45.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="50" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -6809,7 +6809,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>295.59585492227899</v>
       </c>
@@ -6817,7 +6817,7 @@
         <v>8.1640711902113403E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>322.79792746113901</v>
       </c>
@@ -6825,7 +6825,7 @@
         <v>8.0789766407119004E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>373.31606217616502</v>
       </c>
@@ -6833,7 +6833,7 @@
         <v>7.7536151279199106E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>472.79792746113901</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>7.5784204671857605E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>573.05699481865202</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>7.0728587319243599E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>673.31606217616502</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>6.4822024471635098E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>772.79792746114003</v>
       </c>
@@ -6865,7 +6865,7 @@
         <v>5.8014460511679598E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>873.05699481865202</v>
       </c>
@@ -6873,13 +6873,13 @@
         <v>5.0255839822024397E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="156" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="17" t="s">
+    <row r="36" spans="1:2" ht="156" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="17"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="19"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
         <v>5</v>
       </c>
@@ -6907,23 +6907,23 @@
       <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="12.54296875" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="26" width="12.5" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E1" s="19"/>
+    </row>
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -6937,7 +6937,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>296.10389610389598</v>
       </c>
@@ -6952,7 +6952,7 @@
         <v>454.68159000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>322.72727272727201</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>467.34913999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>348.05194805194799</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>488.52064999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>373.376623376623</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>509.65287000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>398.05194805194799</v>
       </c>
@@ -7012,7 +7012,7 @@
         <v>522.20258000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>423.376623376623</v>
       </c>
@@ -7027,7 +7027,7 @@
         <v>543.35445000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>447.402597402597</v>
       </c>
@@ -7042,7 +7042,7 @@
         <v>551.60307999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>472.72727272727201</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>572.75495000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>498.05194805194799</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>585.30466000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>522.72727272727195</v>
       </c>
@@ -7087,7 +7087,7 @@
         <v>610.73796000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>548.05194805194799</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>653.39520000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>572.72727272727195</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>721.85888999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>598.05194805194799</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>803.22581000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>622.72727272727195</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>901.79701999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>648.05194805194799</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>1026.1550500000001</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>673.376623376623</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>583.95378690629002</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>698.05194805194799</v>
       </c>
@@ -7178,7 +7178,7 @@
         <v>597.04749679075701</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>722.72727272727195</v>
       </c>
@@ -7186,7 +7186,7 @@
         <v>611.68164313221996</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>747.40259740259705</v>
       </c>
@@ -7194,7 +7194,7 @@
         <v>628.62644415917805</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>773.376623376623</v>
       </c>
@@ -7202,7 +7202,7 @@
         <v>655.58408215661098</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>797.40259740259705</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>687.16302952503202</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>822.72727272727195</v>
       </c>
@@ -7218,7 +7218,7 @@
         <v>721.05263157894694</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>847.40259740259705</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>764.18485237483901</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>872.72727272727195</v>
       </c>
@@ -7234,20 +7234,20 @@
         <v>801.155327342747</v>
       </c>
     </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="Y36" s="7"/>
     </row>
-    <row r="47" spans="1:25" ht="285" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="17" t="s">
+    <row r="47" spans="1:25" ht="285" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B47" s="17"/>
-      <c r="D47" s="17" t="s">
+      <c r="B47" s="19"/>
+      <c r="D47" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="E47" s="17"/>
-    </row>
-    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="E47" s="19"/>
+    </row>
+    <row r="49" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>5</v>
       </c>
@@ -7255,82 +7255,82 @@
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="F50" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F51" s="2">
         <v>20.54795</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F52" s="2">
         <v>53.424660000000003</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F53" s="2">
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F54" s="2">
         <v>152.05479</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F55" s="2">
         <v>201.36985999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F56" s="2">
         <v>250.68493000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F57" s="2">
         <v>300</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F58" s="2">
         <v>349.31506999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F59" s="2">
         <v>398.63013999999998</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F60" s="2">
         <v>450.68493000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F61" s="2">
         <v>500</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F62" s="2">
         <v>549.31506999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F63" s="2">
         <v>598.63013999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F64" s="2">
         <v>647.94520999999997</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F65" s="2">
         <v>700</v>
       </c>
@@ -7359,23 +7359,23 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="12.54296875" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="8.81640625" style="2"/>
+    <col min="1" max="26" width="12.5" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="3" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="E1" s="19"/>
+    </row>
+    <row r="3" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7389,7 +7389,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>295.83333333333297</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>28.158940000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>322.61904761904702</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>28.887419999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>372.61904761904702</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>29.748339999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>473.21428571428498</v>
       </c>
@@ -7449,7 +7449,7 @@
         <v>30.27815</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>572.61904761904702</v>
       </c>
@@ -7464,7 +7464,7 @@
         <v>30.344370000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>672.61904761904702</v>
       </c>
@@ -7479,7 +7479,7 @@
         <v>30.211919999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>772.61904761904702</v>
       </c>
@@ -7494,7 +7494,7 @@
         <v>29.947019999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>872.61904761904702</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>29.682120000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D12" s="2">
         <f t="shared" si="0"/>
         <v>674.36986000000002</v>
@@ -7518,7 +7518,7 @@
         <v>29.483440000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" s="2">
         <f t="shared" si="0"/>
         <v>723.68493000000001</v>
@@ -7527,7 +7527,7 @@
         <v>29.350989999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D14" s="2">
         <f t="shared" si="0"/>
         <v>775.73973000000001</v>
@@ -7536,7 +7536,7 @@
         <v>29.61589</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D15" s="2">
         <f t="shared" si="0"/>
         <v>825.05479000000003</v>
@@ -7545,7 +7545,7 @@
         <v>30.079470000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D16" s="2">
         <f t="shared" si="0"/>
         <v>874.36986000000002</v>
@@ -7554,17 +7554,17 @@
         <v>31.13907</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="208.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="17" t="s">
+    <row r="33" spans="1:22" ht="208.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="D33" s="17" t="s">
+      <c r="B33" s="19"/>
+      <c r="D33" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="35" spans="1:22" ht="29" x14ac:dyDescent="0.35">
+      <c r="E33" s="19"/>
+    </row>
+    <row r="35" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
         <v>5</v>
       </c>
@@ -7572,73 +7572,73 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" ht="16" x14ac:dyDescent="0.2">
       <c r="D36" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D37" s="2">
         <v>20.54795</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D38" s="2">
         <v>50.684930000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D39" s="2">
         <v>102.73972999999999</v>
       </c>
       <c r="V39" s="7"/>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D40" s="2">
         <v>152.05479</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D41" s="2">
         <v>201.36985999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D42" s="2">
         <v>253.42465999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D43" s="2">
         <v>300</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D44" s="2">
         <v>352.05479000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D45" s="2">
         <v>401.36986000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D46" s="2">
         <v>450.68493000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D47" s="2">
         <v>502.73973000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.2">
       <c r="D48" s="2">
         <v>552.05479000000003</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D49" s="2">
         <v>601.36986000000002</v>
       </c>
@@ -7667,33 +7667,33 @@
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="10" customWidth="1"/>
-    <col min="2" max="2" width="21.81640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" style="10"/>
-    <col min="4" max="4" width="16.453125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="8.81640625" style="10"/>
+    <col min="1" max="1" width="15.5" style="10" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" style="10"/>
+    <col min="4" max="4" width="16.5" style="10" customWidth="1"/>
+    <col min="5" max="5" width="20.5" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="8.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="D1" s="18" t="s">
+      <c r="B1" s="20"/>
+      <c r="D1" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="18"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E1" s="20"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="33" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>303.31797235022998</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>327.64976958525301</v>
       </c>
@@ -7739,7 +7739,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>344.23963133640501</v>
       </c>
@@ -7755,7 +7755,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>365.806451612903</v>
       </c>
@@ -7771,7 +7771,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>396.22119815668202</v>
       </c>
@@ -7787,7 +7787,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>423.31797235022998</v>
       </c>
@@ -7803,7 +7803,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>450.41474654377799</v>
       </c>
@@ -7819,7 +7819,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>467.00460829492999</v>
       </c>
@@ -7835,7 +7835,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>497.41935483870901</v>
       </c>
@@ -7851,7 +7851,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>523.41013824884703</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>545.52995391704997</v>
       </c>
@@ -7883,7 +7883,7 @@
         <v>112.99999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>577.05069124423903</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>601.935483870967</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>657.78801843317899</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>682.11981566820202</v>
       </c>
@@ -7939,7 +7939,7 @@
         <v>96.227544910179603</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>708.11059907834101</v>
       </c>
@@ -7947,7 +7947,7 @@
         <v>99.580838323353206</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>734.65437788018403</v>
       </c>
@@ -7955,7 +7955,7 @@
         <v>102.57485029940101</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>763.41013824884703</v>
       </c>
@@ -7963,7 +7963,7 @@
         <v>105.808383233532</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>783.87096774193503</v>
       </c>
@@ -7971,7 +7971,7 @@
         <v>107.96407185628701</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>817.05069124423903</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>111.19760479041901</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>850.23041474654303</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>114.19161676646701</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <v>883.963133640553</v>
       </c>
@@ -7995,7 +7995,7 @@
         <v>117.425149700598</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
         <v>924.88479262672797</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>121.377245508982</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="D28" s="5" t="s">
         <v>81</v>
       </c>
@@ -8011,7 +8011,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D29">
         <v>20</v>
       </c>
@@ -8019,7 +8019,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D30">
         <v>50</v>
       </c>
@@ -8027,7 +8027,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D31">
         <v>100</v>
       </c>
@@ -8035,7 +8035,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D32">
         <v>150</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D33">
         <v>200</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D34">
         <v>250</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D35">
         <v>300</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D36">
         <v>350</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D37">
         <v>400</v>
       </c>
@@ -8084,7 +8084,7 @@
       </c>
       <c r="V37" s="12"/>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D38">
         <v>450</v>
       </c>
@@ -8092,7 +8092,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D39">
         <v>500</v>
       </c>
@@ -8100,7 +8100,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D40">
         <v>550</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D41">
         <v>600</v>
       </c>
@@ -8116,7 +8116,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.2">
       <c r="D42">
         <v>650</v>
       </c>
@@ -8124,7 +8124,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="45" spans="2:22" ht="232" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:22" ht="224" x14ac:dyDescent="0.2">
       <c r="D45" s="16" t="s">
         <v>78</v>
       </c>
@@ -8135,18 +8135,18 @@
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B46" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="210" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="17" t="s">
+    <row r="53" spans="1:2" ht="210" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B53" s="17"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B53" s="19"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>5</v>
       </c>
@@ -8174,18 +8174,18 @@
       <selection activeCell="A39" sqref="A39:B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="12.54296875" style="2"/>
+    <col min="1" max="16384" width="12.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17"/>
-    </row>
-    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="19"/>
+    </row>
+    <row r="3" spans="1:2" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -8193,7 +8193,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>100</v>
       </c>
@@ -8201,7 +8201,7 @@
         <v>10.6898734177215</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>200</v>
       </c>
@@ -8209,7 +8209,7 @@
         <v>11.0443037974683</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>300</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>11.386075949366999</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>400</v>
       </c>
@@ -8225,7 +8225,7 @@
         <v>11.6962025316455</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>500</v>
       </c>
@@ -8233,7 +8233,7 @@
         <v>11.987341772151799</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>600</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>12.246835443037901</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>700</v>
       </c>
@@ -8249,13 +8249,13 @@
         <v>12.487341772151799</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="187.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="17" t="s">
+    <row r="39" spans="1:2" ht="187.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="17"/>
-    </row>
-    <row r="40" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B39" s="19"/>
+    </row>
+    <row r="40" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>14</v>
       </c>
@@ -8281,27 +8281,27 @@
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="12.54296875" style="2"/>
+    <col min="1" max="16384" width="12.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="19"/>
       <c r="I1" s="11"/>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
@@ -8321,7 +8321,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>473.100871731008</v>
       </c>
@@ -8341,7 +8341,7 @@
         <v>8.3535353535353393E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>573.22540473225399</v>
       </c>
@@ -8361,7 +8361,7 @@
         <v>0.10090909090909</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>672.97633872976303</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>0.12030303030303</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>772.72727272727195</v>
       </c>
@@ -8401,7 +8401,7 @@
         <v>0.14070707070707</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>872.851805728518</v>
       </c>
@@ -8421,11 +8421,11 @@
         <v>0.16292929292929201</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -8440,34 +8440,34 @@
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="1:14" ht="153" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="19" t="s">
+    <row r="33" spans="1:14" ht="153" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="19"/>
+      <c r="B33" s="21"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
       <c r="J33" s="9"/>
-      <c r="K33" s="19" t="s">
+      <c r="K33" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-    </row>
-    <row r="34" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+    </row>
+    <row r="34" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="E35" s="7" t="s">
         <v>103</v>
       </c>
@@ -8498,22 +8498,22 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" style="5" customWidth="1"/>
-    <col min="2" max="16384" width="9.1796875" style="5"/>
+    <col min="1" max="1" width="12.83203125" style="5" customWidth="1"/>
+    <col min="2" max="16384" width="9.1640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="22"/>
       <c r="D1" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>74</v>
       </c>
@@ -8527,7 +8527,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>374.76697420604501</v>
       </c>
@@ -8541,7 +8541,7 @@
         <v>83.230300780628596</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>412.10995015364199</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>81.215235235179406</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>474.554014292452</v>
       </c>
@@ -8569,7 +8569,7 @@
         <v>82.570938959143305</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>540.89825105148998</v>
       </c>
@@ -8583,7 +8583,7 @@
         <v>80.337481614620103</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>603.34231519030095</v>
       </c>
@@ -8597,7 +8597,7 @@
         <v>79.104579669049201</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>668.56250994275695</v>
       </c>
@@ -8611,7 +8611,7 @@
         <v>77.867491299214905</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>732.68797393811303</v>
       </c>
@@ -8625,7 +8625,7 @@
         <v>75.439365226443698</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>793.45330287942204</v>
       </c>
@@ -8639,7 +8639,7 @@
         <v>76.5941205857645</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>858.12146910000195</v>
       </c>
@@ -8653,7 +8653,7 @@
         <v>76.1559415128621</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" s="5">
         <v>920.80490844290102</v>
       </c>
@@ -8661,7 +8661,7 @@
         <v>74.721742333959497</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D14" s="5">
         <v>979.91015480001397</v>
       </c>
@@ -8669,7 +8669,7 @@
         <v>70.899885850165106</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D15" s="5">
         <v>1044.5743240320301</v>
       </c>
@@ -8677,7 +8677,7 @@
         <v>69.265784912685106</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D16" s="5">
         <v>1108.68380007312</v>
       </c>
@@ -8685,7 +8685,7 @@
         <v>67.233624801493704</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D17" s="5">
         <v>1172.2532385480399</v>
       </c>
@@ -8693,7 +8693,7 @@
         <v>62.612161283390201</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D18" s="5">
         <v>1232.4625419689</v>
       </c>
@@ -8701,18 +8701,18 @@
         <v>60.383239231819097</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="179.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="17" t="s">
+    <row r="27" spans="1:5" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B27" s="17"/>
-    </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="C30" s="22" t="s">
+      <c r="B27" s="19"/>
+    </row>
+    <row r="30" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="C30" s="17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" ht="80" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>77</v>
       </c>
@@ -8732,47 +8732,47 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B499B7-5D41-461D-8465-819EE01970F8}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.1796875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="1" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="D1" s="17" t="s">
+      <c r="B1" s="19"/>
+      <c r="D1" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="G1" s="17" t="s">
+      <c r="E1" s="19"/>
+      <c r="G1" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="17"/>
-      <c r="J1" s="17" t="s">
+      <c r="H1" s="19"/>
+      <c r="J1" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="K1" s="17"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -8785,7 +8785,7 @@
       <c r="J2" s="11"/>
       <c r="K2" s="11"/>
     </row>
-    <row r="3" spans="1:11" ht="33.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="42" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -8811,7 +8811,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>20</v>
       </c>
@@ -8837,346 +8837,274 @@
         <v>420.225490196078</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>100</v>
+        <v>650</v>
       </c>
       <c r="B5" s="8">
-        <v>405</v>
+        <v>310.53921568627402</v>
       </c>
       <c r="D5" s="2">
-        <v>100</v>
+        <v>650</v>
       </c>
       <c r="E5" s="8">
-        <v>410</v>
+        <v>309.803921568627</v>
       </c>
       <c r="G5" s="2">
-        <v>100</v>
+        <v>650</v>
       </c>
       <c r="H5" s="8">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+        <v>305.166666666666</v>
+      </c>
+      <c r="J5" s="2">
+        <v>650</v>
+      </c>
+      <c r="K5" s="2">
+        <v>300.225490196078</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>200</v>
+        <v>700</v>
       </c>
       <c r="B6" s="8">
-        <v>400</v>
+        <v>264.70588235294099</v>
       </c>
       <c r="D6" s="2">
-        <v>200</v>
+        <v>700</v>
       </c>
       <c r="E6" s="8">
-        <v>400</v>
+        <v>260.04901960784298</v>
       </c>
       <c r="G6" s="2">
-        <v>200</v>
+        <v>700</v>
       </c>
       <c r="H6" s="8">
-        <v>400</v>
+        <v>264.57843137254901</v>
       </c>
       <c r="J6" s="2">
-        <v>200</v>
-      </c>
-      <c r="K6" s="8">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>700</v>
+      </c>
+      <c r="K6" s="2">
+        <v>255.04901960784301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>350</v>
+        <v>725</v>
       </c>
       <c r="B7" s="8">
-        <v>375</v>
+        <v>237.74509803921501</v>
       </c>
       <c r="D7" s="2">
-        <v>350</v>
+        <v>750</v>
       </c>
       <c r="E7" s="8">
-        <v>390</v>
+        <v>204.90196078431299</v>
       </c>
       <c r="G7" s="2">
-        <v>350</v>
+        <v>750</v>
       </c>
       <c r="H7" s="8">
-        <v>395</v>
+        <v>214.46078431372499</v>
       </c>
       <c r="J7" s="2">
-        <v>350</v>
-      </c>
-      <c r="K7" s="8">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+        <v>750</v>
+      </c>
+      <c r="K7" s="2">
+        <v>210.225490196078</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>650</v>
+        <v>775</v>
       </c>
       <c r="B8" s="8">
-        <v>310.53921568627402</v>
+        <v>204.65686274509801</v>
       </c>
       <c r="D8" s="2">
-        <v>650</v>
+        <v>800</v>
       </c>
       <c r="E8" s="8">
-        <v>309.803921568627</v>
+        <v>195.09803921568599</v>
       </c>
       <c r="G8" s="2">
-        <v>650</v>
+        <v>800</v>
       </c>
       <c r="H8" s="8">
-        <v>305.166666666666</v>
+        <v>199.99019607843101</v>
       </c>
       <c r="J8" s="2">
-        <v>650</v>
+        <v>800</v>
       </c>
       <c r="K8" s="2">
-        <v>300.225490196078</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>199.99019607843101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>700</v>
+        <v>825</v>
       </c>
       <c r="B9" s="8">
-        <v>264.70588235294099</v>
+        <v>234.803921568627</v>
       </c>
       <c r="D9" s="2">
-        <v>700</v>
+        <v>825</v>
       </c>
       <c r="E9" s="8">
-        <v>260.04901960784298</v>
+        <v>179.65686274509801</v>
       </c>
       <c r="G9" s="2">
-        <v>700</v>
+        <v>825</v>
       </c>
       <c r="H9" s="8">
-        <v>264.57843137254901</v>
+        <v>225.04901960784301</v>
       </c>
       <c r="J9" s="2">
-        <v>700</v>
+        <v>825</v>
       </c>
       <c r="K9" s="2">
-        <v>255.04901960784301</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+        <v>202.81372549019599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>725</v>
+        <v>850</v>
       </c>
       <c r="B10" s="8">
-        <v>237.74509803921501</v>
+        <v>299.50980392156799</v>
       </c>
       <c r="D10" s="2">
-        <v>750</v>
+        <v>850</v>
       </c>
       <c r="E10" s="8">
-        <v>204.90196078431299</v>
+        <v>364.70588235294099</v>
       </c>
       <c r="G10" s="2">
-        <v>750</v>
+        <v>850</v>
       </c>
       <c r="H10" s="8">
-        <v>214.46078431372499</v>
+        <v>389.87254901960699</v>
       </c>
       <c r="J10" s="2">
-        <v>750</v>
+        <v>850</v>
       </c>
       <c r="K10" s="2">
-        <v>210.225490196078</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+        <v>394.81372549019602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>775</v>
+        <v>950</v>
       </c>
       <c r="B11" s="8">
-        <v>204.65686274509801</v>
+        <v>410.29411764705799</v>
       </c>
       <c r="D11" s="2">
-        <v>800</v>
+        <v>950</v>
       </c>
       <c r="E11" s="8">
-        <v>195.09803921568599</v>
+        <v>414.950980392156</v>
       </c>
       <c r="G11" s="2">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="H11" s="8">
-        <v>199.99019607843101</v>
+        <v>405.40196078431302</v>
       </c>
       <c r="J11" s="2">
-        <v>800</v>
+        <v>900</v>
       </c>
       <c r="K11" s="2">
-        <v>199.99019607843101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+        <v>410.34313725490199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>825</v>
+        <v>1000</v>
       </c>
       <c r="B12" s="8">
-        <v>234.803921568627</v>
+        <v>415.19607843137197</v>
       </c>
       <c r="D12" s="2">
-        <v>825</v>
+        <v>1000</v>
       </c>
       <c r="E12" s="8">
-        <v>179.65686274509801</v>
-      </c>
-      <c r="G12" s="2">
-        <v>825</v>
-      </c>
-      <c r="H12" s="8">
-        <v>225.04901960784301</v>
-      </c>
-      <c r="J12" s="2">
-        <v>825</v>
-      </c>
-      <c r="K12" s="2">
-        <v>202.81372549019599</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+        <v>419.85294117646998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="B13" s="8">
-        <v>299.50980392156799</v>
+        <v>410.53921568627402</v>
       </c>
       <c r="D13" s="2">
-        <v>850</v>
+        <v>1050</v>
       </c>
       <c r="E13" s="8">
-        <v>364.70588235294099</v>
-      </c>
-      <c r="G13" s="2">
-        <v>850</v>
-      </c>
-      <c r="H13" s="8">
-        <v>389.87254901960699</v>
-      </c>
-      <c r="J13" s="2">
-        <v>850</v>
-      </c>
-      <c r="K13" s="2">
-        <v>394.81372549019602</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+        <v>417.15686274509801</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>950</v>
+        <v>1100</v>
       </c>
       <c r="B14" s="8">
-        <v>410.29411764705799</v>
+        <v>405.14705882352899</v>
       </c>
       <c r="D14" s="2">
-        <v>950</v>
+        <v>1100</v>
       </c>
       <c r="E14" s="8">
-        <v>414.950980392156</v>
-      </c>
-      <c r="G14" s="2">
-        <v>900</v>
-      </c>
-      <c r="H14" s="8">
-        <v>405.40196078431302</v>
-      </c>
-      <c r="J14" s="2">
-        <v>900</v>
-      </c>
-      <c r="K14" s="2">
-        <v>410.34313725490199</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+        <v>414.70588235294099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>1000</v>
+        <v>1150</v>
       </c>
       <c r="B15" s="8">
-        <v>415.19607843137197</v>
+        <v>390.19607843137197</v>
       </c>
       <c r="D15" s="2">
-        <v>1000</v>
+        <v>1150</v>
       </c>
       <c r="E15" s="8">
-        <v>419.85294117646998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="2">
-        <v>1050</v>
-      </c>
-      <c r="B16" s="8">
-        <v>410.53921568627402</v>
-      </c>
-      <c r="D16" s="2">
-        <v>1050</v>
-      </c>
-      <c r="E16" s="8">
-        <v>417.15686274509801</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2">
-        <v>1100</v>
-      </c>
-      <c r="B17" s="8">
-        <v>405.14705882352899</v>
-      </c>
-      <c r="D17" s="2">
-        <v>1100</v>
-      </c>
-      <c r="E17" s="8">
-        <v>414.70588235294099</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2">
-        <v>1150</v>
-      </c>
-      <c r="B18" s="8">
-        <v>390.19607843137197</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1150</v>
-      </c>
-      <c r="E18" s="8">
         <v>394.85294117646998</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="17" t="s">
+    <row r="36" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="17"/>
-      <c r="K39" s="17"/>
-    </row>
-    <row r="41" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B41" s="7" t="s">
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+    </row>
+    <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B38" s="7" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="A36:K36"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B41" r:id="rId1" xr:uid="{6DCBDDF8-4BF4-4722-A0C1-5EADC355F994}"/>
+    <hyperlink ref="B38" r:id="rId1" xr:uid="{6DCBDDF8-4BF4-4722-A0C1-5EADC355F994}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>